<commit_message>
add folder postman and update folder data_processing
</commit_message>
<xml_diff>
--- a/automatic_testing/submission_export.xlsx
+++ b/automatic_testing/submission_export.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian199887/Downloads/github_francistan88/DSA/automatic_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E99C44-7225-C144-8348-3B99188FB021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870AC583-BB32-324D-AE13-8EF779892C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="94">
   <si>
     <t>Date</t>
   </si>
@@ -302,27 +302,6 @@
   </si>
   <si>
     <t>H228000896VA2</t>
-  </si>
-  <si>
-    <t>H228000897VA2</t>
-  </si>
-  <si>
-    <t>H228000906VA2</t>
-  </si>
-  <si>
-    <t>H228000908VA2</t>
-  </si>
-  <si>
-    <t>H228000909VA2</t>
-  </si>
-  <si>
-    <t>H228000910VA2</t>
-  </si>
-  <si>
-    <t>H228000911VA2</t>
-  </si>
-  <si>
-    <t>H228000914VA2</t>
   </si>
 </sst>
 </file>
@@ -396,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -445,8 +424,6 @@
     <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -752,27 +729,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="99" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="99" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="32" defaultRowHeight="28" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="32" style="11"/>
-    <col min="2" max="2" width="32" style="9"/>
-    <col min="3" max="3" width="32" style="12"/>
-    <col min="4" max="4" width="32" style="5"/>
-    <col min="5" max="5" width="32" style="6"/>
-    <col min="6" max="6" width="32" style="7"/>
-    <col min="7" max="7" width="32" style="5"/>
-    <col min="8" max="8" width="32" style="7"/>
-    <col min="9" max="9" width="32" style="5"/>
-    <col min="10" max="10" width="32" style="7"/>
+    <col min="1" max="1" width="25.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.59765625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.19921875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.19921875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28" customHeight="1">
+    <row r="1" spans="1:10" ht="21.75" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -804,7 +781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="28" customHeight="1">
+    <row r="2" spans="1:10" ht="21.75" customHeight="1">
       <c r="A2" s="15"/>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -832,7 +809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28" customHeight="1">
+    <row r="3" spans="1:10" ht="21.75" customHeight="1">
       <c r="A3" s="15"/>
       <c r="C3" s="16"/>
       <c r="D3" s="3"/>
@@ -845,7 +822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28" customHeight="1">
+    <row r="4" spans="1:10" ht="21.75" customHeight="1">
       <c r="A4" s="15"/>
       <c r="C4" s="16">
         <v>930930090909</v>
@@ -870,7 +847,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="28" customHeight="1">
+    <row r="5" spans="1:10" ht="21.75" customHeight="1">
       <c r="A5" s="15"/>
       <c r="C5" s="16">
         <v>970118123456</v>
@@ -895,7 +872,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="28" customHeight="1">
+    <row r="6" spans="1:10" ht="21.75" customHeight="1">
       <c r="A6" s="15"/>
       <c r="C6" s="16"/>
       <c r="D6" s="3"/>
@@ -908,7 +885,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="28" customHeight="1">
+    <row r="7" spans="1:10" ht="21.75" customHeight="1">
       <c r="A7" s="15"/>
       <c r="C7" s="16">
         <v>980513123456</v>
@@ -933,7 +910,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="28" customHeight="1">
+    <row r="8" spans="1:10" ht="21.75" customHeight="1">
       <c r="A8" s="15"/>
       <c r="C8" s="16">
         <v>891007777777</v>
@@ -958,7 +935,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="28" customHeight="1">
+    <row r="9" spans="1:10" ht="21.75" customHeight="1">
       <c r="A9" s="15"/>
       <c r="C9" s="16">
         <v>891007666666</v>
@@ -983,7 +960,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28" customHeight="1">
+    <row r="10" spans="1:10" ht="21.75" customHeight="1">
       <c r="A10" s="15"/>
       <c r="C10" s="16"/>
       <c r="D10" s="3"/>
@@ -994,7 +971,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="28" customHeight="1">
+    <row r="11" spans="1:10" ht="21.75" customHeight="1">
       <c r="A11" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1026,7 +1003,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28" customHeight="1">
+    <row r="12" spans="1:10" ht="21.75" customHeight="1">
       <c r="A12" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1058,7 +1035,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28" customHeight="1">
+    <row r="13" spans="1:10" ht="21.75" customHeight="1">
       <c r="A13" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1090,7 +1067,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28" customHeight="1">
+    <row r="14" spans="1:10" ht="21.75" customHeight="1">
       <c r="A14" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1122,7 +1099,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28" customHeight="1">
+    <row r="15" spans="1:10" ht="21.75" customHeight="1">
       <c r="A15" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1154,7 +1131,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28" customHeight="1">
+    <row r="16" spans="1:10" ht="21.75" customHeight="1">
       <c r="A16" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1186,7 +1163,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="28" customHeight="1">
+    <row r="17" spans="1:10" ht="21.75" customHeight="1">
       <c r="A17" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1218,7 +1195,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="28" customHeight="1">
+    <row r="18" spans="1:10" ht="21.75" customHeight="1">
       <c r="A18" s="15"/>
       <c r="C18" s="16"/>
       <c r="D18" s="3"/>
@@ -1229,7 +1206,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="28" customHeight="1">
+    <row r="19" spans="1:10" ht="21.75" customHeight="1">
       <c r="A19" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1261,7 +1238,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="28" customHeight="1">
+    <row r="20" spans="1:10" ht="21.75" customHeight="1">
       <c r="A20" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1293,7 +1270,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="28" customHeight="1">
+    <row r="21" spans="1:10" ht="21.75" customHeight="1">
       <c r="A21" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1325,7 +1302,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="28" customHeight="1">
+    <row r="22" spans="1:10" ht="21.75" customHeight="1">
       <c r="A22" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1357,7 +1334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="28" customHeight="1">
+    <row r="23" spans="1:10" ht="21.75" customHeight="1">
       <c r="A23" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1389,7 +1366,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="28" customHeight="1">
+    <row r="24" spans="1:10" ht="21.75" customHeight="1">
       <c r="A24" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1421,7 +1398,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="28" customHeight="1">
+    <row r="25" spans="1:10" ht="21.75" customHeight="1">
       <c r="A25" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1453,7 +1430,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="28" customHeight="1">
+    <row r="26" spans="1:10" ht="21.75" customHeight="1">
       <c r="A26" s="4">
         <v>25569.333854166671</v>
       </c>
@@ -1485,7 +1462,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="28" customHeight="1">
+    <row r="27" spans="1:10" ht="21.75" customHeight="1">
       <c r="A27" s="4"/>
       <c r="B27" s="1"/>
       <c r="C27" s="16"/>
@@ -1497,7 +1474,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" ht="28" customHeight="1">
+    <row r="28" spans="1:10" ht="21.75" customHeight="1">
       <c r="A28" s="13">
         <v>44771</v>
       </c>
@@ -1529,7 +1506,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="28" customHeight="1">
+    <row r="29" spans="1:10" ht="21.75" customHeight="1">
       <c r="A29" s="13">
         <v>44771</v>
       </c>
@@ -1561,7 +1538,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="28" customHeight="1">
+    <row r="30" spans="1:10" ht="21.75" customHeight="1">
       <c r="A30" s="13">
         <v>44771</v>
       </c>
@@ -1593,7 +1570,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="28" customHeight="1">
+    <row r="31" spans="1:10" ht="21.75" customHeight="1">
       <c r="A31" s="13"/>
       <c r="C31" s="16"/>
       <c r="D31" s="3"/>
@@ -1604,7 +1581,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" ht="28" customHeight="1">
+    <row r="32" spans="1:10" ht="21.75" customHeight="1">
       <c r="A32" s="13">
         <v>44775</v>
       </c>
@@ -1636,7 +1613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="28" customHeight="1">
+    <row r="33" spans="1:10" ht="21.75" customHeight="1">
       <c r="A33" s="13">
         <v>44775</v>
       </c>
@@ -1668,7 +1645,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="28" customHeight="1">
+    <row r="34" spans="1:10" ht="21.75" customHeight="1">
       <c r="A34" s="13">
         <v>44775</v>
       </c>
@@ -1700,7 +1677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="28" customHeight="1">
+    <row r="35" spans="1:10" ht="21.75" customHeight="1">
       <c r="A35" s="13">
         <v>44775</v>
       </c>
@@ -1732,7 +1709,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="28" customHeight="1">
+    <row r="36" spans="1:10" ht="21.75" customHeight="1">
       <c r="A36" s="13">
         <v>44775</v>
       </c>
@@ -1764,7 +1741,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="28" customHeight="1">
+    <row r="37" spans="1:10" ht="21.75" customHeight="1">
       <c r="A37" s="13">
         <v>44775</v>
       </c>
@@ -1796,7 +1773,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="28" customHeight="1">
+    <row r="38" spans="1:10" ht="17.25" customHeight="1"/>
+    <row r="39" spans="1:10" ht="21.75" customHeight="1">
       <c r="A39" s="13">
         <v>44776</v>
       </c>
@@ -1828,7 +1806,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="28" customHeight="1">
+    <row r="40" spans="1:10" ht="15" customHeight="1">
       <c r="A40" s="13">
         <v>44776</v>
       </c>
@@ -1860,7 +1838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="28" customHeight="1">
+    <row r="41" spans="1:10">
       <c r="A41" s="17">
         <v>44776</v>
       </c>
@@ -1892,7 +1870,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="28" customHeight="1">
+    <row r="42" spans="1:10">
       <c r="A42" s="17">
         <v>44776</v>
       </c>
@@ -1924,7 +1902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="28" customHeight="1">
+    <row r="43" spans="1:10">
       <c r="A43" s="17">
         <v>44776</v>
       </c>
@@ -1956,7 +1934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="28" customHeight="1">
+    <row r="44" spans="1:10">
       <c r="A44" s="17">
         <v>44776</v>
       </c>
@@ -1988,7 +1966,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="28" customHeight="1">
+    <row r="45" spans="1:10">
       <c r="A45" s="17">
         <v>44776</v>
       </c>
@@ -2020,7 +1998,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="28" customHeight="1">
+    <row r="47" spans="1:10">
       <c r="A47" s="17">
         <v>44777</v>
       </c>
@@ -2052,7 +2030,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="28" customHeight="1">
+    <row r="48" spans="1:10">
       <c r="A48" s="17">
         <v>44777</v>
       </c>
@@ -2084,7 +2062,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="28" customHeight="1">
+    <row r="49" spans="1:10">
       <c r="A49" s="17">
         <v>44777</v>
       </c>
@@ -2116,7 +2094,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="28" customHeight="1">
+    <row r="50" spans="1:10">
       <c r="A50" s="17">
         <v>44777</v>
       </c>
@@ -2148,7 +2126,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="28" customHeight="1">
+    <row r="51" spans="1:10">
       <c r="A51" s="17">
         <v>44777</v>
       </c>
@@ -2180,7 +2158,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="28" customHeight="1">
+    <row r="52" spans="1:10">
       <c r="A52" s="17">
         <v>44777</v>
       </c>
@@ -2212,7 +2190,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="28" customHeight="1">
+    <row r="53" spans="1:10">
       <c r="A53" s="17">
         <v>44777</v>
       </c>
@@ -2244,7 +2222,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="28" customHeight="1">
+    <row r="55" spans="1:10">
       <c r="A55" s="19">
         <v>44777</v>
       </c>
@@ -2276,7 +2254,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="28" customHeight="1">
+    <row r="56" spans="1:10">
       <c r="A56" s="17">
         <v>44777</v>
       </c>
@@ -2308,7 +2286,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="28" customHeight="1">
+    <row r="57" spans="1:10">
       <c r="A57" s="17">
         <v>44777</v>
       </c>
@@ -2340,7 +2318,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="28" customHeight="1">
+    <row r="58" spans="1:10">
       <c r="A58" s="17">
         <v>44777</v>
       </c>
@@ -2372,10 +2350,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="10" customFormat="1" ht="28" customHeight="1">
+    <row r="59" spans="1:10" s="10" customFormat="1">
       <c r="A59" s="20"/>
     </row>
-    <row r="60" spans="1:10" ht="28" customHeight="1">
+    <row r="60" spans="1:10">
       <c r="A60" s="17">
         <v>44778</v>
       </c>
@@ -2407,8 +2385,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="28" customHeight="1">
-      <c r="A61" s="17">
+    <row r="61" spans="1:10">
+      <c r="A61" s="21">
         <v>44778</v>
       </c>
       <c r="B61" t="s">
@@ -2433,236 +2411,9 @@
         <v>17</v>
       </c>
       <c r="I61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J61" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="28" customHeight="1">
-      <c r="A62" s="21">
-        <v>44778</v>
-      </c>
-      <c r="B62" t="s">
-        <v>94</v>
-      </c>
-      <c r="C62" t="s">
-        <v>77</v>
-      </c>
-      <c r="D62" t="s">
-        <v>78</v>
-      </c>
-      <c r="E62" t="s">
-        <v>31</v>
-      </c>
-      <c r="F62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G62" t="s">
-        <v>52</v>
-      </c>
-      <c r="H62" t="s">
-        <v>17</v>
-      </c>
-      <c r="I62">
-        <v>1</v>
-      </c>
-      <c r="J62" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" s="23" customFormat="1" ht="28" customHeight="1">
-      <c r="A63" s="22"/>
-    </row>
-    <row r="64" spans="1:10" ht="28" customHeight="1">
-      <c r="A64" s="21">
-        <v>44781</v>
-      </c>
-      <c r="B64" t="s">
-        <v>96</v>
-      </c>
-      <c r="C64" t="s">
-        <v>66</v>
-      </c>
-      <c r="D64" t="s">
-        <v>67</v>
-      </c>
-      <c r="E64" t="s">
-        <v>68</v>
-      </c>
-      <c r="F64" t="s">
-        <v>19</v>
-      </c>
-      <c r="G64" t="s">
-        <v>69</v>
-      </c>
-      <c r="H64" t="s">
-        <v>20</v>
-      </c>
-      <c r="I64">
-        <v>1</v>
-      </c>
-      <c r="J64" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" s="9" customFormat="1" ht="28" customHeight="1">
-      <c r="A65" s="21">
-        <v>44781</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G65" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H65" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I65" s="9">
-        <v>1</v>
-      </c>
-      <c r="J65" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" s="9" customFormat="1" ht="28" customHeight="1">
-      <c r="A66" s="21">
-        <v>44781</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G66" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H66" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I66" s="9">
-        <v>1</v>
-      </c>
-      <c r="J66" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" s="9" customFormat="1" ht="28" customHeight="1">
-      <c r="A67" s="21">
-        <v>44781</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H67" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I67" s="9">
-        <v>1</v>
-      </c>
-      <c r="J67" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" s="9" customFormat="1" ht="28" customHeight="1">
-      <c r="A68" s="21">
-        <v>44781</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C68" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G68" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H68" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I68" s="9">
-        <v>1</v>
-      </c>
-      <c r="J68" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="28" customHeight="1">
-      <c r="A69" s="21">
-        <v>44781</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G69" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H69" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I69" s="9">
-        <v>1</v>
-      </c>
-      <c r="J69" s="9" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>